<commit_message>
created a Shiny app hoping to publish this map but I cannot make it work everything except the plain old script is a total mess and doesn't work luckily all i need for now is the script
</commit_message>
<xml_diff>
--- a/Nyckelharpa_Origins/NyckelharpaHistoryData2.xlsx
+++ b/Nyckelharpa_Origins/NyckelharpaHistoryData2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\Documents\R\Nyckelharpa\Nyckelharpa_Origins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E229C2-B2D6-4E1B-863F-D0B4907C8B44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC375E7-D44D-4600-886B-43C28D41BEB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
@@ -266,9 +266,6 @@
     <t>1619 CE</t>
   </si>
   <si>
-    <t>images/kallunge_carving.jpg</t>
-  </si>
-  <si>
     <t>images/moraharpa.jpg</t>
   </si>
   <si>
@@ -287,124 +284,127 @@
     <t>images/Schluesselfidel.jpg</t>
   </si>
   <si>
+    <t>images/vefsen.png</t>
+  </si>
+  <si>
+    <t>Image Source</t>
+  </si>
+  <si>
+    <t>Magnus Holmström</t>
+  </si>
+  <si>
+    <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>images/sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>Wikimedia Commons</t>
+  </si>
+  <si>
+    <t>By User:pincopallino - Own work, Public Domain</t>
+  </si>
+  <si>
+    <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
+  </si>
+  <si>
+    <t>images/ESI.jpg</t>
+  </si>
+  <si>
+    <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
+  </si>
+  <si>
+    <t>Angel on a fresco on the ceiling of the Palazzo Pubblico (town hall) by Taddeo di Bartolo</t>
+  </si>
+  <si>
+    <t>1830 CE</t>
+  </si>
+  <si>
+    <t>https://olovjohansson.se/nyckelharpa/</t>
+  </si>
+  <si>
+    <t>1498 CE</t>
+  </si>
+  <si>
+    <t>Lagga church outside of Uppsala</t>
+  </si>
+  <si>
+    <t>images/lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>Olov Johansson</t>
+  </si>
+  <si>
+    <t>1960 CE</t>
+  </si>
+  <si>
+    <t>www.ericsahlstrom.se</t>
+  </si>
+  <si>
+    <t>images/eric.jpg</t>
+  </si>
+  <si>
+    <t>http://esitobo.org/eng/</t>
+  </si>
+  <si>
+    <t>Eric Sahlström-institutet</t>
+  </si>
+  <si>
+    <t>Eric Sahlström, from Göksby, begins rescuing the nyckelharpa from obscurity</t>
+  </si>
+  <si>
+    <t>Wood dates back to 1526 but was the instrument assembled later? We'll never know! This instrument is in the Zorn museum in Mora. Shaped more like a lute.</t>
+  </si>
+  <si>
+    <t>Vefsen harpa. Currently in Musik Museum in Stockholm.</t>
+  </si>
+  <si>
+    <t>Esseharpa, shaped more like a nyckelharpa than its predecessor, the Moraharpa</t>
+  </si>
+  <si>
+    <t>Kontrabasharpa! This was the type of nyckelharpa that Byss-Calle (1783-1847), one of the all-time greatest nyckelharpa players, used.</t>
+  </si>
+  <si>
+    <t>Silverbasharpa- plays best in C major. Invented and played the most in Tierp, aka the Tierpsharpa. Named for the use of a silver-wrapped gut string for the bass string to get more sound.</t>
+  </si>
+  <si>
+    <t>Schlüsselfideln- German word for Nyckelharpa</t>
+  </si>
+  <si>
+    <t>Sigtuna key! https://nyckelharpansforum.net/sigtunanyckel.htm</t>
+  </si>
+  <si>
+    <t>Two angels with nyckelharpa at Tolfta church</t>
+  </si>
+  <si>
+    <t>public domain</t>
+  </si>
+  <si>
+    <t>American Nyckelharpa Association</t>
+  </si>
+  <si>
+    <t>1930 CE</t>
+  </si>
+  <si>
+    <t>August Bohlin wanted to play with fiddlers, so he made it so there were 3 rows of keys and fully chromatic.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
+  </si>
+  <si>
+    <t>images/bohlin.jpeg</t>
+  </si>
+  <si>
+    <t>Sandberg, Paul/Upplandsmuseet</t>
+  </si>
+  <si>
     <t>images/Strohfiddel.jpg</t>
   </si>
   <si>
-    <t>images/vefsen.png</t>
-  </si>
-  <si>
-    <t>Image Source</t>
-  </si>
-  <si>
-    <t>Magnus Holmström</t>
-  </si>
-  <si>
-    <t>https://nyckelharpansforum.net/sigtunanyckel.htm</t>
-  </si>
-  <si>
-    <t>images/sigtuna.jpg</t>
-  </si>
-  <si>
-    <t>Wikimedia Commons</t>
-  </si>
-  <si>
-    <t>By User:pincopallino - Own work, Public Domain</t>
-  </si>
-  <si>
-    <t>http://musikforskning.se/stmonline/vol_9/ternhag/ex1.jpg</t>
-  </si>
-  <si>
-    <t>images/ESI.jpg</t>
-  </si>
-  <si>
-    <t>Oldest representation of the nyckelharpa is on the KällungeChurch in Gotland, Sweden.</t>
-  </si>
-  <si>
-    <t>Angel on a fresco on the ceiling of the Palazzo Pubblico (town hall) by Taddeo di Bartolo</t>
-  </si>
-  <si>
-    <t>1830 CE</t>
-  </si>
-  <si>
-    <t>https://olovjohansson.se/nyckelharpa/</t>
-  </si>
-  <si>
-    <t>1498 CE</t>
-  </si>
-  <si>
-    <t>Lagga church outside of Uppsala</t>
-  </si>
-  <si>
-    <t>images/Silverbasharpa.jpg</t>
-  </si>
-  <si>
-    <t>images/lagga-600.jpg</t>
-  </si>
-  <si>
-    <t>Olov Johansson</t>
-  </si>
-  <si>
-    <t>1960 CE</t>
-  </si>
-  <si>
-    <t>www.ericsahlstrom.se</t>
-  </si>
-  <si>
-    <t>images/eric.jpg</t>
-  </si>
-  <si>
-    <t>http://esitobo.org/eng/</t>
-  </si>
-  <si>
-    <t>Eric Sahlström-institutet</t>
-  </si>
-  <si>
-    <t>Eric Sahlström, from Göksby, begins rescuing the nyckelharpa from obscurity</t>
-  </si>
-  <si>
-    <t>Wood dates back to 1526 but was the instrument assembled later? We'll never know! This instrument is in the Zorn museum in Mora. Shaped more like a lute.</t>
-  </si>
-  <si>
-    <t>Vefsen harpa. Currently in Musik Museum in Stockholm.</t>
-  </si>
-  <si>
-    <t>Esseharpa, shaped more like a nyckelharpa than its predecessor, the Moraharpa</t>
-  </si>
-  <si>
-    <t>Kontrabasharpa! This was the type of nyckelharpa that Byss-Calle (1783-1847), one of the all-time greatest nyckelharpa players, used.</t>
-  </si>
-  <si>
-    <t>Silverbasharpa- plays best in C major. Invented and played the most in Tierp, aka the Tierpsharpa. Named for the use of a silver-wrapped gut string for the bass string to get more sound.</t>
-  </si>
-  <si>
-    <t>Schlüsselfideln- German word for Nyckelharpa</t>
-  </si>
-  <si>
-    <t>Sigtuna key! https://nyckelharpansforum.net/sigtunanyckel.htm</t>
-  </si>
-  <si>
-    <t>Two angels with nyckelharpa at Tolfta church</t>
-  </si>
-  <si>
-    <t>public domain</t>
-  </si>
-  <si>
-    <t>American Nyckelharpa Association</t>
-  </si>
-  <si>
-    <t>1930 CE</t>
-  </si>
-  <si>
-    <t>August Bohlin wanted to play with fiddlers, so he made it so there were 3 rows of keys and fully chromatic.</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/August_Bohlin</t>
-  </si>
-  <si>
-    <t>images/bohlin.jpeg</t>
-  </si>
-  <si>
-    <t>Sandberg, Paul/Upplandsmuseet</t>
+    <t>www/Silverbasharpa.jpg</t>
+  </si>
+  <si>
+    <t>www/kallunge_carving.jpg</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H1" t="s">
         <v>64</v>
@@ -867,16 +867,16 @@
         <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="I2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,16 +896,16 @@
         <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,16 +925,16 @@
         <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -954,16 +954,16 @@
         <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,16 +983,16 @@
         <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1012,16 +1012,16 @@
         <v>71</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1044,13 +1044,13 @@
         <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1070,16 +1070,16 @@
         <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1099,16 +1099,16 @@
         <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1128,16 +1128,16 @@
         <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1163,10 +1163,10 @@
         <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1183,19 +1183,19 @@
         <v>17.484182700000002</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1212,19 +1212,19 @@
         <v>17.828809799999998</v>
       </c>
       <c r="E14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" t="s">
         <v>98</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>99</v>
-      </c>
-      <c r="G14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,19 +1241,19 @@
         <v>17.7290031</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1270,19 +1270,19 @@
         <v>17.773121499999998</v>
       </c>
       <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
         <v>119</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>120</v>
-      </c>
-      <c r="G16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H16" t="s">
-        <v>122</v>
-      </c>
-      <c r="I16" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>